<commit_message>
Recurso modificado por presencia de ecuaciones
Archivos actualizados
</commit_message>
<xml_diff>
--- a/fuentes/visuales/grado10/guion02/SolicitudGrafica_CN_10_02_CO.xlsx
+++ b/fuentes/visuales/grado10/guion02/SolicitudGrafica_CN_10_02_CO.xlsx
@@ -1638,6 +1638,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1722,9 +1725,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2475,8 +2475,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2514,14 +2514,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="F2" s="82" t="s">
+      <c r="D2" s="91"/>
+      <c r="F2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="83"/>
+      <c r="G2" s="84"/>
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
       <c r="J2" s="16"/>
@@ -2531,14 +2531,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="91">
+      <c r="C3" s="92">
         <v>10</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="F3" s="84">
+      <c r="D3" s="93"/>
+      <c r="F3" s="85">
         <v>42065</v>
       </c>
-      <c r="G3" s="85"/>
+      <c r="G3" s="86"/>
       <c r="H3" s="50"/>
       <c r="I3" s="50"/>
       <c r="J3" s="16"/>
@@ -2548,10 +2548,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="5"/>
       <c r="F4" s="49" t="s">
         <v>55</v>
@@ -2569,10 +2569,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="95" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="95"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="5"/>
       <c r="F5" s="47" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2620,12 +2620,12 @@
       <c r="B8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="89"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2686,17 +2686,17 @@
       <c r="E10" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="F10" s="14" t="e">
-        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE(#REF!,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G10" s="14" t="e">
+      <c r="F10" s="14" t="str">
+        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v>CN_10_02_CO_IMG01_small</v>
+      </c>
+      <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H10" s="14" t="e">
-        <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE(#REF!,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H10" s="14" t="str">
+        <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v>CN_10_02_CO_IMG01_zoom</v>
       </c>
       <c r="I10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2724,17 +2724,17 @@
       <c r="E11" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="14" t="e">
-        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(#REF!,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G11" s="14" t="e">
+      <c r="F11" s="14" t="str">
+        <f t="shared" ref="F11:F74" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v>CN_10_02_CO_IMG02_small</v>
+      </c>
+      <c r="G11" s="14" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H11" s="14" t="e">
-        <f>IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(#REF!,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H11" s="14" t="str">
+        <f t="shared" ref="H11:H74" si="1">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v>CN_10_02_CO_IMG02_zoom</v>
       </c>
       <c r="I11" s="14" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2755,7 +2755,7 @@
         <v>176</v>
       </c>
       <c r="C12" s="74" t="str">
-        <f t="shared" ref="C12:C21" si="0">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C12:C21" si="2">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -2764,17 +2764,17 @@
       <c r="E12" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F12" s="14" t="e">
-        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(#REF!,"_",$A12,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I12="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G12" s="14" t="e">
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG03_small</v>
+      </c>
+      <c r="G12" s="14" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H12" s="14" t="e">
-        <f>IF(AND(I12&lt;&gt;"",I12&lt;&gt;0),IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(#REF!,"_",$A12,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H12" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG03_zoom</v>
       </c>
       <c r="I12" s="14" t="str">
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2793,7 +2793,7 @@
         <v>177</v>
       </c>
       <c r="C13" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -2802,17 +2802,17 @@
       <c r="E13" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="14" t="e">
-        <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),CONCATENATE(#REF!,"_",$A13,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I13="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G13" s="14" t="e">
+      <c r="F13" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG04_small</v>
+      </c>
+      <c r="G13" s="14" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="14" t="e">
-        <f>IF(AND(I13&lt;&gt;"",I13&lt;&gt;0),IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),CONCATENATE(#REF!,"_",$A13,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H13" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG04_zoom</v>
       </c>
       <c r="I13" s="14" t="str">
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2831,7 +2831,7 @@
         <v>179</v>
       </c>
       <c r="C14" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
@@ -2840,17 +2840,17 @@
       <c r="E14" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="14" t="e">
-        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(#REF!,"_",$A14,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I14="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G14" s="14" t="e">
+      <c r="F14" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG05_small</v>
+      </c>
+      <c r="G14" s="14" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H14" s="14" t="e">
-        <f>IF(AND(I14&lt;&gt;"",I14&lt;&gt;0),IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(#REF!,"_",$A14,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H14" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG05_zoom</v>
       </c>
       <c r="I14" s="14" t="str">
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2869,7 +2869,7 @@
         <v>180</v>
       </c>
       <c r="C15" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -2878,17 +2878,17 @@
       <c r="E15" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="14" t="e">
-        <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),CONCATENATE(#REF!,"_",$A15,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I15="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G15" s="14" t="e">
+      <c r="F15" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG06_small</v>
+      </c>
+      <c r="G15" s="14" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="14" t="e">
-        <f>IF(AND(I15&lt;&gt;"",I15&lt;&gt;0),IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),CONCATENATE(#REF!,"_",$A15,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H15" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG06_zoom</v>
       </c>
       <c r="I15" s="14" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2909,7 +2909,7 @@
         <v>180</v>
       </c>
       <c r="C16" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -2918,17 +2918,17 @@
       <c r="E16" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="14" t="e">
-        <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE(#REF!,"_",$A16,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I16="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G16" s="14" t="e">
+      <c r="F16" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG07_small</v>
+      </c>
+      <c r="G16" s="14" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H16" s="14" t="e">
-        <f>IF(AND(I16&lt;&gt;"",I16&lt;&gt;0),IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE(#REF!,"_",$A16,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H16" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG07_zoom</v>
       </c>
       <c r="I16" s="14" t="str">
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2949,7 +2949,7 @@
         <v>187</v>
       </c>
       <c r="C17" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -2958,17 +2958,17 @@
       <c r="E17" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="14" t="e">
-        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE(#REF!,"_",$A17,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I17="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G17" s="14" t="e">
+      <c r="F17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG08_small</v>
+      </c>
+      <c r="G17" s="14" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H17" s="14" t="e">
-        <f>IF(AND(I17&lt;&gt;"",I17&lt;&gt;0),IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE(#REF!,"_",$A17,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H17" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG08_zoom</v>
       </c>
       <c r="I17" s="14" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2989,7 +2989,7 @@
         <v>188</v>
       </c>
       <c r="C18" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -2998,17 +2998,17 @@
       <c r="E18" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F18" s="14" t="e">
-        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE(#REF!,"_",$A18,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I18="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G18" s="14" t="e">
+      <c r="F18" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG09_small</v>
+      </c>
+      <c r="G18" s="14" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H18" s="14" t="e">
-        <f>IF(AND(I18&lt;&gt;"",I18&lt;&gt;0),IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE(#REF!,"_",$A18,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H18" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG09_zoom</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3027,7 +3027,7 @@
         <v>190</v>
       </c>
       <c r="C19" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -3036,17 +3036,17 @@
       <c r="E19" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F19" s="14" t="e">
-        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(#REF!,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G19" s="14" t="e">
+      <c r="F19" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG10_small</v>
+      </c>
+      <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H19" s="14" t="e">
-        <f>IF(AND(I19&lt;&gt;"",I19&lt;&gt;0),IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(#REF!,"_",$A19,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H19" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3067,7 +3067,7 @@
         <v>190</v>
       </c>
       <c r="C20" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -3076,17 +3076,17 @@
       <c r="E20" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F20" s="14" t="e">
-        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(#REF!,"_",$A20,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I20="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G20" s="14" t="e">
+      <c r="F20" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG11_small</v>
+      </c>
+      <c r="G20" s="14" t="str">
         <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H20" s="14" t="e">
-        <f>IF(AND(I20&lt;&gt;"",I20&lt;&gt;0),IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(#REF!,"_",$A20,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H20" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG11_zoom</v>
       </c>
       <c r="I20" s="14" t="str">
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3107,7 +3107,7 @@
         <v>193</v>
       </c>
       <c r="C21" s="74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -3116,17 +3116,17 @@
       <c r="E21" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F21" s="14" t="e">
-        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE(#REF!,"_",$A21,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I21="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G21" s="14" t="e">
+      <c r="F21" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG12_small</v>
+      </c>
+      <c r="G21" s="14" t="str">
         <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H21" s="14" t="e">
-        <f>IF(AND(I21&lt;&gt;"",I21&lt;&gt;0),IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE(#REF!,"_",$A21,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H21" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG12_zoom</v>
       </c>
       <c r="I21" s="14" t="str">
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3147,7 +3147,7 @@
         <v>196</v>
       </c>
       <c r="C22" s="74" t="str">
-        <f t="shared" ref="C22:C27" si="1">IF(OR(B21&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C22:C27" si="3">IF(OR(B21&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="14" t="s">
@@ -3156,17 +3156,17 @@
       <c r="E22" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="14" t="e">
-        <f>IF(OR(B21&lt;&gt;"",J22&lt;&gt;""),CONCATENATE(#REF!,"_",$A22,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I22="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G22" s="14" t="e">
+      <c r="F22" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG13_small</v>
+      </c>
+      <c r="G22" s="14" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H22" s="14" t="e">
-        <f>IF(AND(I22&lt;&gt;"",I22&lt;&gt;0),IF(OR(B21&lt;&gt;"",J22&lt;&gt;""),CONCATENATE(#REF!,"_",$A22,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H22" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG13_zoom</v>
       </c>
       <c r="I22" s="14" t="str">
         <f>IF(OR(B21&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3185,7 +3185,7 @@
         <v>196</v>
       </c>
       <c r="C23" s="74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="14" t="s">
@@ -3194,17 +3194,17 @@
       <c r="E23" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F23" s="14" t="e">
-        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),CONCATENATE(#REF!,"_",$A23,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I23="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G23" s="14" t="e">
+      <c r="F23" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG14_small</v>
+      </c>
+      <c r="G23" s="14" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H23" s="14" t="e">
-        <f>IF(AND(I23&lt;&gt;"",I23&lt;&gt;0),IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),CONCATENATE(#REF!,"_",$A23,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H23" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG14_zoom</v>
       </c>
       <c r="I23" s="14" t="str">
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3223,7 +3223,7 @@
         <v>199</v>
       </c>
       <c r="C24" s="74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="14" t="s">
@@ -3232,17 +3232,17 @@
       <c r="E24" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="14" t="e">
-        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE(#REF!,"_",$A24,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I24="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G24" s="14" t="e">
+      <c r="F24" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG15_small</v>
+      </c>
+      <c r="G24" s="14" t="str">
         <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H24" s="14" t="e">
-        <f>IF(AND(I24&lt;&gt;"",I24&lt;&gt;0),IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE(#REF!,"_",$A24,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H24" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG15_zoom</v>
       </c>
       <c r="I24" s="14" t="str">
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3261,7 +3261,7 @@
         <v>200</v>
       </c>
       <c r="C25" s="74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="14" t="s">
@@ -3270,17 +3270,17 @@
       <c r="E25" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F25" s="14" t="e">
-        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),CONCATENATE(#REF!,"_",$A25,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I25="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G25" s="14" t="e">
+      <c r="F25" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG16_small</v>
+      </c>
+      <c r="G25" s="14" t="str">
         <f>IF(F25&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H25" s="14" t="e">
-        <f>IF(AND(I25&lt;&gt;"",I25&lt;&gt;0),IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),CONCATENATE(#REF!,"_",$A25,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H25" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG16_zoom</v>
       </c>
       <c r="I25" s="14" t="str">
         <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3299,7 +3299,7 @@
         <v>202</v>
       </c>
       <c r="C26" s="74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -3308,17 +3308,17 @@
       <c r="E26" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="14" t="e">
-        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE(#REF!,"_",$A26,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I26="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G26" s="14" t="e">
+      <c r="F26" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG17_small</v>
+      </c>
+      <c r="G26" s="14" t="str">
         <f>IF(F26&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H26" s="14" t="e">
-        <f>IF(AND(I26&lt;&gt;"",I26&lt;&gt;0),IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE(#REF!,"_",$A26,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H26" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG17_zoom</v>
       </c>
       <c r="I26" s="14" t="str">
         <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3337,7 +3337,7 @@
         <v>204</v>
       </c>
       <c r="C27" s="74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D27" s="14" t="s">
@@ -3346,17 +3346,17 @@
       <c r="E27" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="14" t="e">
-        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),CONCATENATE(#REF!,"_",$A27,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I27="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G27" s="14" t="e">
+      <c r="F27" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG18_small</v>
+      </c>
+      <c r="G27" s="14" t="str">
         <f>IF(F27&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H27" s="14" t="e">
-        <f>IF(AND(I27&lt;&gt;"",I27&lt;&gt;0),IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),CONCATENATE(#REF!,"_",$A27,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H27" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG18_zoom</v>
       </c>
       <c r="I27" s="14" t="str">
         <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3371,23 +3371,23 @@
       <c r="A28" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="114" t="s">
+      <c r="B28" s="82" t="s">
         <v>206</v>
       </c>
       <c r="C28" s="74"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="14" t="e">
-        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),CONCATENATE(#REF!,"_",$A28,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I28="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G28" s="14" t="e">
+      <c r="F28" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>CN_10_02_CO_IMG19_small</v>
+      </c>
+      <c r="G28" s="14" t="str">
         <f>IF(F28&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H28" s="14" t="e">
-        <f>IF(AND(I28&lt;&gt;"",I28&lt;&gt;0),IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),CONCATENATE(#REF!,"_",$A28,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H28" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CN_10_02_CO_IMG19_zoom</v>
       </c>
       <c r="I28" s="14" t="str">
         <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3403,7 +3403,7 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14" t="str">
-        <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),CONCATENATE(#REF!,"_",$A29,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I29="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G29" s="14" t="str">
@@ -3411,7 +3411,7 @@
         <v/>
       </c>
       <c r="H29" s="14" t="str">
-        <f>IF(AND(I29&lt;&gt;"",I29&lt;&gt;0),IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),CONCATENATE(#REF!,"_",$A29,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I29" s="14" t="str">
@@ -3428,7 +3428,7 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14" t="str">
-        <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),CONCATENATE(#REF!,"_",$A30,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I30="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G30" s="14" t="str">
@@ -3436,7 +3436,7 @@
         <v/>
       </c>
       <c r="H30" s="14" t="str">
-        <f>IF(AND(I30&lt;&gt;"",I30&lt;&gt;0),IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),CONCATENATE(#REF!,"_",$A30,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I30" s="14" t="str">
@@ -3453,7 +3453,7 @@
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14" t="str">
-        <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),CONCATENATE(#REF!,"_",$A31,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I31="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G31" s="14" t="str">
@@ -3461,7 +3461,7 @@
         <v/>
       </c>
       <c r="H31" s="14" t="str">
-        <f>IF(AND(I31&lt;&gt;"",I31&lt;&gt;0),IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),CONCATENATE(#REF!,"_",$A31,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I31" s="14" t="str">
@@ -3478,7 +3478,7 @@
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14" t="str">
-        <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),CONCATENATE(#REF!,"_",$A32,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I32="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G32" s="14" t="str">
@@ -3486,7 +3486,7 @@
         <v/>
       </c>
       <c r="H32" s="14" t="str">
-        <f>IF(AND(I32&lt;&gt;"",I32&lt;&gt;0),IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),CONCATENATE(#REF!,"_",$A32,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I32" s="14" t="str">
@@ -3503,7 +3503,7 @@
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14" t="str">
-        <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),CONCATENATE(#REF!,"_",$A33,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I33="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G33" s="14" t="str">
@@ -3511,7 +3511,7 @@
         <v/>
       </c>
       <c r="H33" s="14" t="str">
-        <f>IF(AND(I33&lt;&gt;"",I33&lt;&gt;0),IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),CONCATENATE(#REF!,"_",$A33,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I33" s="14" t="str">
@@ -3528,7 +3528,7 @@
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14" t="str">
-        <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(#REF!,"_",$A34,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I34="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G34" s="14" t="str">
@@ -3536,7 +3536,7 @@
         <v/>
       </c>
       <c r="H34" s="14" t="str">
-        <f>IF(AND(I34&lt;&gt;"",I34&lt;&gt;0),IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(#REF!,"_",$A34,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I34" s="14" t="str">
@@ -3553,7 +3553,7 @@
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14" t="str">
-        <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),CONCATENATE(#REF!,"_",$A35,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I35="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G35" s="14" t="str">
@@ -3561,7 +3561,7 @@
         <v/>
       </c>
       <c r="H35" s="14" t="str">
-        <f>IF(AND(I35&lt;&gt;"",I35&lt;&gt;0),IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),CONCATENATE(#REF!,"_",$A35,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I35" s="14" t="str">
@@ -3578,7 +3578,7 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14" t="str">
-        <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE(#REF!,"_",$A36,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I36="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G36" s="14" t="str">
@@ -3586,7 +3586,7 @@
         <v/>
       </c>
       <c r="H36" s="14" t="str">
-        <f>IF(AND(I36&lt;&gt;"",I36&lt;&gt;0),IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE(#REF!,"_",$A36,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I36" s="14" t="str">
@@ -3603,7 +3603,7 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14" t="str">
-        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),CONCATENATE(#REF!,"_",$A37,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I37="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G37" s="14" t="str">
@@ -3611,7 +3611,7 @@
         <v/>
       </c>
       <c r="H37" s="14" t="str">
-        <f>IF(AND(I37&lt;&gt;"",I37&lt;&gt;0),IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),CONCATENATE(#REF!,"_",$A37,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I37" s="14" t="str">
@@ -3628,7 +3628,7 @@
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14" t="str">
-        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),CONCATENATE(#REF!,"_",$A38,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I38="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G38" s="14" t="str">
@@ -3636,7 +3636,7 @@
         <v/>
       </c>
       <c r="H38" s="14" t="str">
-        <f>IF(AND(I38&lt;&gt;"",I38&lt;&gt;0),IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),CONCATENATE(#REF!,"_",$A38,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I38" s="14" t="str">
@@ -3653,7 +3653,7 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14" t="str">
-        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),CONCATENATE(#REF!,"_",$A39,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I39="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G39" s="14" t="str">
@@ -3661,7 +3661,7 @@
         <v/>
       </c>
       <c r="H39" s="14" t="str">
-        <f>IF(AND(I39&lt;&gt;"",I39&lt;&gt;0),IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),CONCATENATE(#REF!,"_",$A39,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I39" s="14" t="str">
@@ -3678,7 +3678,7 @@
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14" t="str">
-        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),CONCATENATE(#REF!,"_",$A40,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I40="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G40" s="14" t="str">
@@ -3686,7 +3686,7 @@
         <v/>
       </c>
       <c r="H40" s="14" t="str">
-        <f>IF(AND(I40&lt;&gt;"",I40&lt;&gt;0),IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),CONCATENATE(#REF!,"_",$A40,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I40" s="14" t="str">
@@ -3703,7 +3703,7 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14" t="str">
-        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE(#REF!,"_",$A41,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I41="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G41" s="14" t="str">
@@ -3711,7 +3711,7 @@
         <v/>
       </c>
       <c r="H41" s="14" t="str">
-        <f>IF(AND(I41&lt;&gt;"",I41&lt;&gt;0),IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE(#REF!,"_",$A41,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I41" s="14" t="str">
@@ -3728,7 +3728,7 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="str">
-        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),CONCATENATE(#REF!,"_",$A42,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I42="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G42" s="14" t="str">
@@ -3736,7 +3736,7 @@
         <v/>
       </c>
       <c r="H42" s="14" t="str">
-        <f>IF(AND(I42&lt;&gt;"",I42&lt;&gt;0),IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),CONCATENATE(#REF!,"_",$A42,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I42" s="14" t="str">
@@ -3753,7 +3753,7 @@
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14" t="str">
-        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),CONCATENATE(#REF!,"_",$A43,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I43="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G43" s="14" t="str">
@@ -3761,7 +3761,7 @@
         <v/>
       </c>
       <c r="H43" s="14" t="str">
-        <f>IF(AND(I43&lt;&gt;"",I43&lt;&gt;0),IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),CONCATENATE(#REF!,"_",$A43,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I43" s="14" t="str">
@@ -3778,7 +3778,7 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14" t="str">
-        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),CONCATENATE(#REF!,"_",$A44,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I44="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G44" s="14" t="str">
@@ -3786,7 +3786,7 @@
         <v/>
       </c>
       <c r="H44" s="14" t="str">
-        <f>IF(AND(I44&lt;&gt;"",I44&lt;&gt;0),IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),CONCATENATE(#REF!,"_",$A44,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I44" s="14" t="str">
@@ -3803,7 +3803,7 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14" t="str">
-        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),CONCATENATE(#REF!,"_",$A45,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I45="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G45" s="14" t="str">
@@ -3811,7 +3811,7 @@
         <v/>
       </c>
       <c r="H45" s="14" t="str">
-        <f>IF(AND(I45&lt;&gt;"",I45&lt;&gt;0),IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),CONCATENATE(#REF!,"_",$A45,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I45" s="14" t="str">
@@ -3828,7 +3828,7 @@
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14" t="str">
-        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),CONCATENATE(#REF!,"_",$A46,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I46="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G46" s="14" t="str">
@@ -3836,7 +3836,7 @@
         <v/>
       </c>
       <c r="H46" s="14" t="str">
-        <f>IF(AND(I46&lt;&gt;"",I46&lt;&gt;0),IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),CONCATENATE(#REF!,"_",$A46,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I46" s="14" t="str">
@@ -3853,7 +3853,7 @@
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14" t="str">
-        <f>IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),CONCATENATE(#REF!,"_",$A47,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I47="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G47" s="14" t="str">
@@ -3861,7 +3861,7 @@
         <v/>
       </c>
       <c r="H47" s="14" t="str">
-        <f>IF(AND(I47&lt;&gt;"",I47&lt;&gt;0),IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),CONCATENATE(#REF!,"_",$A47,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I47" s="14" t="str">
@@ -3878,7 +3878,7 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14" t="str">
-        <f>IF(OR(B48&lt;&gt;"",J48&lt;&gt;""),CONCATENATE(#REF!,"_",$A48,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I48="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G48" s="14" t="str">
@@ -3886,7 +3886,7 @@
         <v/>
       </c>
       <c r="H48" s="14" t="str">
-        <f>IF(AND(I48&lt;&gt;"",I48&lt;&gt;0),IF(OR(B48&lt;&gt;"",J48&lt;&gt;""),CONCATENATE(#REF!,"_",$A48,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I48" s="14" t="str">
@@ -3903,7 +3903,7 @@
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14" t="str">
-        <f>IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),CONCATENATE(#REF!,"_",$A49,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I49="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G49" s="14" t="str">
@@ -3911,7 +3911,7 @@
         <v/>
       </c>
       <c r="H49" s="14" t="str">
-        <f>IF(AND(I49&lt;&gt;"",I49&lt;&gt;0),IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),CONCATENATE(#REF!,"_",$A49,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I49" s="14" t="str">
@@ -3928,7 +3928,7 @@
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14" t="str">
-        <f>IF(OR(B50&lt;&gt;"",J50&lt;&gt;""),CONCATENATE(#REF!,"_",$A50,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I50="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G50" s="14" t="str">
@@ -3936,7 +3936,7 @@
         <v/>
       </c>
       <c r="H50" s="14" t="str">
-        <f>IF(AND(I50&lt;&gt;"",I50&lt;&gt;0),IF(OR(B50&lt;&gt;"",J50&lt;&gt;""),CONCATENATE(#REF!,"_",$A50,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I50" s="14" t="str">
@@ -3953,7 +3953,7 @@
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14" t="str">
-        <f>IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(#REF!,"_",$A51,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I51="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G51" s="14" t="str">
@@ -3961,7 +3961,7 @@
         <v/>
       </c>
       <c r="H51" s="14" t="str">
-        <f>IF(AND(I51&lt;&gt;"",I51&lt;&gt;0),IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(#REF!,"_",$A51,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I51" s="14" t="str">
@@ -3978,7 +3978,7 @@
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14" t="str">
-        <f>IF(OR(B52&lt;&gt;"",J52&lt;&gt;""),CONCATENATE(#REF!,"_",$A52,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I52="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G52" s="14" t="str">
@@ -3986,7 +3986,7 @@
         <v/>
       </c>
       <c r="H52" s="14" t="str">
-        <f>IF(AND(I52&lt;&gt;"",I52&lt;&gt;0),IF(OR(B52&lt;&gt;"",J52&lt;&gt;""),CONCATENATE(#REF!,"_",$A52,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I52" s="14" t="str">
@@ -4003,7 +4003,7 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14" t="str">
-        <f>IF(OR(B53&lt;&gt;"",J53&lt;&gt;""),CONCATENATE(#REF!,"_",$A53,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I53="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G53" s="14" t="str">
@@ -4011,7 +4011,7 @@
         <v/>
       </c>
       <c r="H53" s="14" t="str">
-        <f>IF(AND(I53&lt;&gt;"",I53&lt;&gt;0),IF(OR(B53&lt;&gt;"",J53&lt;&gt;""),CONCATENATE(#REF!,"_",$A53,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I53" s="14" t="str">
@@ -4028,7 +4028,7 @@
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14" t="str">
-        <f>IF(OR(B54&lt;&gt;"",J54&lt;&gt;""),CONCATENATE(#REF!,"_",$A54,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I54="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G54" s="14" t="str">
@@ -4036,7 +4036,7 @@
         <v/>
       </c>
       <c r="H54" s="14" t="str">
-        <f>IF(AND(I54&lt;&gt;"",I54&lt;&gt;0),IF(OR(B54&lt;&gt;"",J54&lt;&gt;""),CONCATENATE(#REF!,"_",$A54,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I54" s="14" t="str">
@@ -4053,7 +4053,7 @@
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14" t="str">
-        <f>IF(OR(B55&lt;&gt;"",J55&lt;&gt;""),CONCATENATE(#REF!,"_",$A55,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I55="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G55" s="14" t="str">
@@ -4061,7 +4061,7 @@
         <v/>
       </c>
       <c r="H55" s="14" t="str">
-        <f>IF(AND(I55&lt;&gt;"",I55&lt;&gt;0),IF(OR(B55&lt;&gt;"",J55&lt;&gt;""),CONCATENATE(#REF!,"_",$A55,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I55" s="14" t="str">
@@ -4078,7 +4078,7 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14" t="str">
-        <f>IF(OR(B56&lt;&gt;"",J56&lt;&gt;""),CONCATENATE(#REF!,"_",$A56,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I56="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G56" s="14" t="str">
@@ -4086,7 +4086,7 @@
         <v/>
       </c>
       <c r="H56" s="14" t="str">
-        <f>IF(AND(I56&lt;&gt;"",I56&lt;&gt;0),IF(OR(B56&lt;&gt;"",J56&lt;&gt;""),CONCATENATE(#REF!,"_",$A56,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I56" s="14" t="str">
@@ -4103,7 +4103,7 @@
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14" t="str">
-        <f>IF(OR(B57&lt;&gt;"",J57&lt;&gt;""),CONCATENATE(#REF!,"_",$A57,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I57="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G57" s="14" t="str">
@@ -4111,7 +4111,7 @@
         <v/>
       </c>
       <c r="H57" s="14" t="str">
-        <f>IF(AND(I57&lt;&gt;"",I57&lt;&gt;0),IF(OR(B57&lt;&gt;"",J57&lt;&gt;""),CONCATENATE(#REF!,"_",$A57,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I57" s="14" t="str">
@@ -4128,7 +4128,7 @@
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14" t="str">
-        <f>IF(OR(B58&lt;&gt;"",J58&lt;&gt;""),CONCATENATE(#REF!,"_",$A58,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I58="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G58" s="14" t="str">
@@ -4136,7 +4136,7 @@
         <v/>
       </c>
       <c r="H58" s="14" t="str">
-        <f>IF(AND(I58&lt;&gt;"",I58&lt;&gt;0),IF(OR(B58&lt;&gt;"",J58&lt;&gt;""),CONCATENATE(#REF!,"_",$A58,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I58" s="14" t="str">
@@ -4153,7 +4153,7 @@
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14" t="str">
-        <f>IF(OR(B59&lt;&gt;"",J59&lt;&gt;""),CONCATENATE(#REF!,"_",$A59,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I59="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G59" s="14" t="str">
@@ -4161,7 +4161,7 @@
         <v/>
       </c>
       <c r="H59" s="14" t="str">
-        <f>IF(AND(I59&lt;&gt;"",I59&lt;&gt;0),IF(OR(B59&lt;&gt;"",J59&lt;&gt;""),CONCATENATE(#REF!,"_",$A59,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I59" s="14" t="str">
@@ -4178,7 +4178,7 @@
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14" t="str">
-        <f>IF(OR(B60&lt;&gt;"",J60&lt;&gt;""),CONCATENATE(#REF!,"_",$A60,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I60="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G60" s="14" t="str">
@@ -4186,7 +4186,7 @@
         <v/>
       </c>
       <c r="H60" s="14" t="str">
-        <f>IF(AND(I60&lt;&gt;"",I60&lt;&gt;0),IF(OR(B60&lt;&gt;"",J60&lt;&gt;""),CONCATENATE(#REF!,"_",$A60,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I60" s="14" t="str">
@@ -4203,7 +4203,7 @@
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14" t="str">
-        <f>IF(OR(B61&lt;&gt;"",J61&lt;&gt;""),CONCATENATE(#REF!,"_",$A61,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I61="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G61" s="14" t="str">
@@ -4211,7 +4211,7 @@
         <v/>
       </c>
       <c r="H61" s="14" t="str">
-        <f>IF(AND(I61&lt;&gt;"",I61&lt;&gt;0),IF(OR(B61&lt;&gt;"",J61&lt;&gt;""),CONCATENATE(#REF!,"_",$A61,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I61" s="14" t="str">
@@ -4228,7 +4228,7 @@
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14" t="str">
-        <f>IF(OR(B62&lt;&gt;"",J62&lt;&gt;""),CONCATENATE(#REF!,"_",$A62,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I62="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G62" s="14" t="str">
@@ -4236,7 +4236,7 @@
         <v/>
       </c>
       <c r="H62" s="14" t="str">
-        <f>IF(AND(I62&lt;&gt;"",I62&lt;&gt;0),IF(OR(B62&lt;&gt;"",J62&lt;&gt;""),CONCATENATE(#REF!,"_",$A62,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I62" s="14" t="str">
@@ -4253,7 +4253,7 @@
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14" t="str">
-        <f>IF(OR(B63&lt;&gt;"",J63&lt;&gt;""),CONCATENATE(#REF!,"_",$A63,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I63="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G63" s="14" t="str">
@@ -4261,7 +4261,7 @@
         <v/>
       </c>
       <c r="H63" s="14" t="str">
-        <f>IF(AND(I63&lt;&gt;"",I63&lt;&gt;0),IF(OR(B63&lt;&gt;"",J63&lt;&gt;""),CONCATENATE(#REF!,"_",$A63,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I63" s="14" t="str">
@@ -4278,7 +4278,7 @@
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14" t="str">
-        <f>IF(OR(B64&lt;&gt;"",J64&lt;&gt;""),CONCATENATE(#REF!,"_",$A64,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I64="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G64" s="14" t="str">
@@ -4286,7 +4286,7 @@
         <v/>
       </c>
       <c r="H64" s="14" t="str">
-        <f>IF(AND(I64&lt;&gt;"",I64&lt;&gt;0),IF(OR(B64&lt;&gt;"",J64&lt;&gt;""),CONCATENATE(#REF!,"_",$A64,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I64" s="14" t="str">
@@ -4303,7 +4303,7 @@
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="14" t="str">
-        <f>IF(OR(B65&lt;&gt;"",J65&lt;&gt;""),CONCATENATE(#REF!,"_",$A65,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I65="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G65" s="14" t="str">
@@ -4311,7 +4311,7 @@
         <v/>
       </c>
       <c r="H65" s="14" t="str">
-        <f>IF(AND(I65&lt;&gt;"",I65&lt;&gt;0),IF(OR(B65&lt;&gt;"",J65&lt;&gt;""),CONCATENATE(#REF!,"_",$A65,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I65" s="14" t="str">
@@ -4328,7 +4328,7 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14" t="str">
-        <f>IF(OR(B66&lt;&gt;"",J66&lt;&gt;""),CONCATENATE(#REF!,"_",$A66,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I66="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G66" s="14" t="str">
@@ -4336,7 +4336,7 @@
         <v/>
       </c>
       <c r="H66" s="14" t="str">
-        <f>IF(AND(I66&lt;&gt;"",I66&lt;&gt;0),IF(OR(B66&lt;&gt;"",J66&lt;&gt;""),CONCATENATE(#REF!,"_",$A66,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I66" s="14" t="str">
@@ -4353,7 +4353,7 @@
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14" t="str">
-        <f>IF(OR(B67&lt;&gt;"",J67&lt;&gt;""),CONCATENATE(#REF!,"_",$A67,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I67="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G67" s="14" t="str">
@@ -4361,7 +4361,7 @@
         <v/>
       </c>
       <c r="H67" s="14" t="str">
-        <f>IF(AND(I67&lt;&gt;"",I67&lt;&gt;0),IF(OR(B67&lt;&gt;"",J67&lt;&gt;""),CONCATENATE(#REF!,"_",$A67,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I67" s="14" t="str">
@@ -4378,7 +4378,7 @@
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14" t="str">
-        <f>IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),CONCATENATE(#REF!,"_",$A68,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I68="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G68" s="14" t="str">
@@ -4386,7 +4386,7 @@
         <v/>
       </c>
       <c r="H68" s="14" t="str">
-        <f>IF(AND(I68&lt;&gt;"",I68&lt;&gt;0),IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),CONCATENATE(#REF!,"_",$A68,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I68" s="14" t="str">
@@ -4403,7 +4403,7 @@
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14" t="str">
-        <f>IF(OR(B69&lt;&gt;"",J69&lt;&gt;""),CONCATENATE(#REF!,"_",$A69,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I69="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G69" s="14" t="str">
@@ -4411,7 +4411,7 @@
         <v/>
       </c>
       <c r="H69" s="14" t="str">
-        <f>IF(AND(I69&lt;&gt;"",I69&lt;&gt;0),IF(OR(B69&lt;&gt;"",J69&lt;&gt;""),CONCATENATE(#REF!,"_",$A69,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I69" s="14" t="str">
@@ -4428,7 +4428,7 @@
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14" t="str">
-        <f>IF(OR(B70&lt;&gt;"",J70&lt;&gt;""),CONCATENATE(#REF!,"_",$A70,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I70="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G70" s="14" t="str">
@@ -4436,7 +4436,7 @@
         <v/>
       </c>
       <c r="H70" s="14" t="str">
-        <f>IF(AND(I70&lt;&gt;"",I70&lt;&gt;0),IF(OR(B70&lt;&gt;"",J70&lt;&gt;""),CONCATENATE(#REF!,"_",$A70,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I70" s="14" t="str">
@@ -4453,7 +4453,7 @@
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14" t="str">
-        <f>IF(OR(B71&lt;&gt;"",J71&lt;&gt;""),CONCATENATE(#REF!,"_",$A71,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I71="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G71" s="14" t="str">
@@ -4461,7 +4461,7 @@
         <v/>
       </c>
       <c r="H71" s="14" t="str">
-        <f>IF(AND(I71&lt;&gt;"",I71&lt;&gt;0),IF(OR(B71&lt;&gt;"",J71&lt;&gt;""),CONCATENATE(#REF!,"_",$A71,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I71" s="14" t="str">
@@ -4478,7 +4478,7 @@
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14" t="str">
-        <f>IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),CONCATENATE(#REF!,"_",$A72,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I72="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G72" s="14" t="str">
@@ -4486,7 +4486,7 @@
         <v/>
       </c>
       <c r="H72" s="14" t="str">
-        <f>IF(AND(I72&lt;&gt;"",I72&lt;&gt;0),IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),CONCATENATE(#REF!,"_",$A72,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I72" s="14" t="str">
@@ -4503,7 +4503,7 @@
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14" t="str">
-        <f>IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),CONCATENATE(#REF!,"_",$A73,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I73="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G73" s="14" t="str">
@@ -4511,7 +4511,7 @@
         <v/>
       </c>
       <c r="H73" s="14" t="str">
-        <f>IF(AND(I73&lt;&gt;"",I73&lt;&gt;0),IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),CONCATENATE(#REF!,"_",$A73,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I73" s="14" t="str">
@@ -4528,7 +4528,7 @@
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14" t="str">
-        <f>IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),CONCATENATE(#REF!,"_",$A74,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I74="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G74" s="14" t="str">
@@ -4536,7 +4536,7 @@
         <v/>
       </c>
       <c r="H74" s="14" t="str">
-        <f>IF(AND(I74&lt;&gt;"",I74&lt;&gt;0),IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),CONCATENATE(#REF!,"_",$A74,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I74" s="14" t="str">
@@ -4553,7 +4553,7 @@
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="14" t="str">
-        <f>IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE(#REF!,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F75:F108" si="4">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G75" s="14" t="str">
@@ -4561,7 +4561,7 @@
         <v/>
       </c>
       <c r="H75" s="14" t="str">
-        <f>IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE(#REF!,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H75:H108" si="5">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I75" s="14" t="str">
@@ -4578,7 +4578,7 @@
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="14" t="str">
-        <f>IF(OR(B76&lt;&gt;"",J76&lt;&gt;""),CONCATENATE(#REF!,"_",$A76,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I76="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G76" s="14" t="str">
@@ -4586,7 +4586,7 @@
         <v/>
       </c>
       <c r="H76" s="14" t="str">
-        <f>IF(AND(I76&lt;&gt;"",I76&lt;&gt;0),IF(OR(B76&lt;&gt;"",J76&lt;&gt;""),CONCATENATE(#REF!,"_",$A76,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I76" s="14" t="str">
@@ -4603,7 +4603,7 @@
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="14" t="str">
-        <f>IF(OR(B77&lt;&gt;"",J77&lt;&gt;""),CONCATENATE(#REF!,"_",$A77,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I77="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G77" s="14" t="str">
@@ -4611,7 +4611,7 @@
         <v/>
       </c>
       <c r="H77" s="14" t="str">
-        <f>IF(AND(I77&lt;&gt;"",I77&lt;&gt;0),IF(OR(B77&lt;&gt;"",J77&lt;&gt;""),CONCATENATE(#REF!,"_",$A77,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I77" s="14" t="str">
@@ -4628,7 +4628,7 @@
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="14" t="str">
-        <f>IF(OR(B78&lt;&gt;"",J78&lt;&gt;""),CONCATENATE(#REF!,"_",$A78,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I78="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G78" s="14" t="str">
@@ -4636,7 +4636,7 @@
         <v/>
       </c>
       <c r="H78" s="14" t="str">
-        <f>IF(AND(I78&lt;&gt;"",I78&lt;&gt;0),IF(OR(B78&lt;&gt;"",J78&lt;&gt;""),CONCATENATE(#REF!,"_",$A78,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I78" s="14" t="str">
@@ -4653,7 +4653,7 @@
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="14" t="str">
-        <f>IF(OR(B79&lt;&gt;"",J79&lt;&gt;""),CONCATENATE(#REF!,"_",$A79,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I79="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G79" s="14" t="str">
@@ -4661,7 +4661,7 @@
         <v/>
       </c>
       <c r="H79" s="14" t="str">
-        <f>IF(AND(I79&lt;&gt;"",I79&lt;&gt;0),IF(OR(B79&lt;&gt;"",J79&lt;&gt;""),CONCATENATE(#REF!,"_",$A79,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I79" s="14" t="str">
@@ -4678,7 +4678,7 @@
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="14" t="str">
-        <f>IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),CONCATENATE(#REF!,"_",$A80,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I80="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G80" s="14" t="str">
@@ -4686,7 +4686,7 @@
         <v/>
       </c>
       <c r="H80" s="14" t="str">
-        <f>IF(AND(I80&lt;&gt;"",I80&lt;&gt;0),IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),CONCATENATE(#REF!,"_",$A80,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I80" s="14" t="str">
@@ -4703,7 +4703,7 @@
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="14" t="str">
-        <f>IF(OR(B81&lt;&gt;"",J81&lt;&gt;""),CONCATENATE(#REF!,"_",$A81,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I81="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G81" s="14" t="str">
@@ -4711,7 +4711,7 @@
         <v/>
       </c>
       <c r="H81" s="14" t="str">
-        <f>IF(AND(I81&lt;&gt;"",I81&lt;&gt;0),IF(OR(B81&lt;&gt;"",J81&lt;&gt;""),CONCATENATE(#REF!,"_",$A81,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I81" s="14" t="str">
@@ -4728,7 +4728,7 @@
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="14" t="str">
-        <f>IF(OR(B82&lt;&gt;"",J82&lt;&gt;""),CONCATENATE(#REF!,"_",$A82,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I82="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G82" s="14" t="str">
@@ -4736,7 +4736,7 @@
         <v/>
       </c>
       <c r="H82" s="14" t="str">
-        <f>IF(AND(I82&lt;&gt;"",I82&lt;&gt;0),IF(OR(B82&lt;&gt;"",J82&lt;&gt;""),CONCATENATE(#REF!,"_",$A82,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I82" s="14" t="str">
@@ -4753,7 +4753,7 @@
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="14" t="str">
-        <f>IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(#REF!,"_",$A83,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I83="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G83" s="14" t="str">
@@ -4761,7 +4761,7 @@
         <v/>
       </c>
       <c r="H83" s="14" t="str">
-        <f>IF(AND(I83&lt;&gt;"",I83&lt;&gt;0),IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(#REF!,"_",$A83,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I83" s="14" t="str">
@@ -4778,7 +4778,7 @@
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="14" t="str">
-        <f>IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(#REF!,"_",$A84,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I84="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G84" s="14" t="str">
@@ -4786,7 +4786,7 @@
         <v/>
       </c>
       <c r="H84" s="14" t="str">
-        <f>IF(AND(I84&lt;&gt;"",I84&lt;&gt;0),IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(#REF!,"_",$A84,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I84" s="14" t="str">
@@ -4803,7 +4803,7 @@
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="14" t="str">
-        <f>IF(OR(B85&lt;&gt;"",J85&lt;&gt;""),CONCATENATE(#REF!,"_",$A85,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I85="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G85" s="14" t="str">
@@ -4811,7 +4811,7 @@
         <v/>
       </c>
       <c r="H85" s="14" t="str">
-        <f>IF(AND(I85&lt;&gt;"",I85&lt;&gt;0),IF(OR(B85&lt;&gt;"",J85&lt;&gt;""),CONCATENATE(#REF!,"_",$A85,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I85" s="14" t="str">
@@ -4828,7 +4828,7 @@
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="14" t="str">
-        <f>IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),CONCATENATE(#REF!,"_",$A86,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I86="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G86" s="14" t="str">
@@ -4836,7 +4836,7 @@
         <v/>
       </c>
       <c r="H86" s="14" t="str">
-        <f>IF(AND(I86&lt;&gt;"",I86&lt;&gt;0),IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),CONCATENATE(#REF!,"_",$A86,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I86" s="14" t="str">
@@ -4853,7 +4853,7 @@
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="14" t="str">
-        <f>IF(OR(B87&lt;&gt;"",J87&lt;&gt;""),CONCATENATE(#REF!,"_",$A87,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I87="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G87" s="14" t="str">
@@ -4861,7 +4861,7 @@
         <v/>
       </c>
       <c r="H87" s="14" t="str">
-        <f>IF(AND(I87&lt;&gt;"",I87&lt;&gt;0),IF(OR(B87&lt;&gt;"",J87&lt;&gt;""),CONCATENATE(#REF!,"_",$A87,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I87" s="14" t="str">
@@ -4878,7 +4878,7 @@
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="14" t="str">
-        <f>IF(OR(B88&lt;&gt;"",J88&lt;&gt;""),CONCATENATE(#REF!,"_",$A88,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I88="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G88" s="14" t="str">
@@ -4886,7 +4886,7 @@
         <v/>
       </c>
       <c r="H88" s="14" t="str">
-        <f>IF(AND(I88&lt;&gt;"",I88&lt;&gt;0),IF(OR(B88&lt;&gt;"",J88&lt;&gt;""),CONCATENATE(#REF!,"_",$A88,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I88" s="14" t="str">
@@ -4903,7 +4903,7 @@
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="14" t="str">
-        <f>IF(OR(B89&lt;&gt;"",J89&lt;&gt;""),CONCATENATE(#REF!,"_",$A89,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I89="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G89" s="14" t="str">
@@ -4911,7 +4911,7 @@
         <v/>
       </c>
       <c r="H89" s="14" t="str">
-        <f>IF(AND(I89&lt;&gt;"",I89&lt;&gt;0),IF(OR(B89&lt;&gt;"",J89&lt;&gt;""),CONCATENATE(#REF!,"_",$A89,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I89" s="14" t="str">
@@ -4928,7 +4928,7 @@
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="14" t="str">
-        <f>IF(OR(B90&lt;&gt;"",J90&lt;&gt;""),CONCATENATE(#REF!,"_",$A90,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I90="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G90" s="14" t="str">
@@ -4936,7 +4936,7 @@
         <v/>
       </c>
       <c r="H90" s="14" t="str">
-        <f>IF(AND(I90&lt;&gt;"",I90&lt;&gt;0),IF(OR(B90&lt;&gt;"",J90&lt;&gt;""),CONCATENATE(#REF!,"_",$A90,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I90" s="14" t="str">
@@ -4953,7 +4953,7 @@
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="14" t="str">
-        <f>IF(OR(B91&lt;&gt;"",J91&lt;&gt;""),CONCATENATE(#REF!,"_",$A91,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I91="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G91" s="14" t="str">
@@ -4961,7 +4961,7 @@
         <v/>
       </c>
       <c r="H91" s="14" t="str">
-        <f>IF(AND(I91&lt;&gt;"",I91&lt;&gt;0),IF(OR(B91&lt;&gt;"",J91&lt;&gt;""),CONCATENATE(#REF!,"_",$A91,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I91" s="14" t="str">
@@ -4978,7 +4978,7 @@
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="14" t="str">
-        <f>IF(OR(B92&lt;&gt;"",J92&lt;&gt;""),CONCATENATE(#REF!,"_",$A92,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I92="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G92" s="14" t="str">
@@ -4986,7 +4986,7 @@
         <v/>
       </c>
       <c r="H92" s="14" t="str">
-        <f>IF(AND(I92&lt;&gt;"",I92&lt;&gt;0),IF(OR(B92&lt;&gt;"",J92&lt;&gt;""),CONCATENATE(#REF!,"_",$A92,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I92" s="14" t="str">
@@ -5003,7 +5003,7 @@
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="14" t="str">
-        <f>IF(OR(B93&lt;&gt;"",J93&lt;&gt;""),CONCATENATE(#REF!,"_",$A93,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I93="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G93" s="14" t="str">
@@ -5011,7 +5011,7 @@
         <v/>
       </c>
       <c r="H93" s="14" t="str">
-        <f>IF(AND(I93&lt;&gt;"",I93&lt;&gt;0),IF(OR(B93&lt;&gt;"",J93&lt;&gt;""),CONCATENATE(#REF!,"_",$A93,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I93" s="14" t="str">
@@ -5028,7 +5028,7 @@
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="14" t="str">
-        <f>IF(OR(B94&lt;&gt;"",J94&lt;&gt;""),CONCATENATE(#REF!,"_",$A94,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I94="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G94" s="14" t="str">
@@ -5036,7 +5036,7 @@
         <v/>
       </c>
       <c r="H94" s="14" t="str">
-        <f>IF(AND(I94&lt;&gt;"",I94&lt;&gt;0),IF(OR(B94&lt;&gt;"",J94&lt;&gt;""),CONCATENATE(#REF!,"_",$A94,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I94" s="14" t="str">
@@ -5053,7 +5053,7 @@
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="14" t="str">
-        <f>IF(OR(B95&lt;&gt;"",J95&lt;&gt;""),CONCATENATE(#REF!,"_",$A95,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I95="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G95" s="14" t="str">
@@ -5061,7 +5061,7 @@
         <v/>
       </c>
       <c r="H95" s="14" t="str">
-        <f>IF(AND(I95&lt;&gt;"",I95&lt;&gt;0),IF(OR(B95&lt;&gt;"",J95&lt;&gt;""),CONCATENATE(#REF!,"_",$A95,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I95" s="14" t="str">
@@ -5078,7 +5078,7 @@
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="14" t="str">
-        <f>IF(OR(B96&lt;&gt;"",J96&lt;&gt;""),CONCATENATE(#REF!,"_",$A96,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I96="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G96" s="14" t="str">
@@ -5086,7 +5086,7 @@
         <v/>
       </c>
       <c r="H96" s="14" t="str">
-        <f>IF(AND(I96&lt;&gt;"",I96&lt;&gt;0),IF(OR(B96&lt;&gt;"",J96&lt;&gt;""),CONCATENATE(#REF!,"_",$A96,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I96" s="14" t="str">
@@ -5103,7 +5103,7 @@
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="14" t="str">
-        <f>IF(OR(B97&lt;&gt;"",J97&lt;&gt;""),CONCATENATE(#REF!,"_",$A97,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I97="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G97" s="14" t="str">
@@ -5111,7 +5111,7 @@
         <v/>
       </c>
       <c r="H97" s="14" t="str">
-        <f>IF(AND(I97&lt;&gt;"",I97&lt;&gt;0),IF(OR(B97&lt;&gt;"",J97&lt;&gt;""),CONCATENATE(#REF!,"_",$A97,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I97" s="14" t="str">
@@ -5128,7 +5128,7 @@
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="14" t="str">
-        <f>IF(OR(B98&lt;&gt;"",J98&lt;&gt;""),CONCATENATE(#REF!,"_",$A98,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I98="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G98" s="14" t="str">
@@ -5136,7 +5136,7 @@
         <v/>
       </c>
       <c r="H98" s="14" t="str">
-        <f>IF(AND(I98&lt;&gt;"",I98&lt;&gt;0),IF(OR(B98&lt;&gt;"",J98&lt;&gt;""),CONCATENATE(#REF!,"_",$A98,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I98" s="14" t="str">
@@ -5153,7 +5153,7 @@
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
       <c r="F99" s="14" t="str">
-        <f>IF(OR(B99&lt;&gt;"",J99&lt;&gt;""),CONCATENATE(#REF!,"_",$A99,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I99="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G99" s="14" t="str">
@@ -5161,7 +5161,7 @@
         <v/>
       </c>
       <c r="H99" s="14" t="str">
-        <f>IF(AND(I99&lt;&gt;"",I99&lt;&gt;0),IF(OR(B99&lt;&gt;"",J99&lt;&gt;""),CONCATENATE(#REF!,"_",$A99,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I99" s="14" t="str">
@@ -5178,7 +5178,7 @@
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
       <c r="F100" s="14" t="str">
-        <f>IF(OR(B100&lt;&gt;"",J100&lt;&gt;""),CONCATENATE(#REF!,"_",$A100,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I100="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G100" s="14" t="str">
@@ -5186,7 +5186,7 @@
         <v/>
       </c>
       <c r="H100" s="14" t="str">
-        <f>IF(AND(I100&lt;&gt;"",I100&lt;&gt;0),IF(OR(B100&lt;&gt;"",J100&lt;&gt;""),CONCATENATE(#REF!,"_",$A100,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I100" s="14" t="str">
@@ -5203,7 +5203,7 @@
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="str">
-        <f>IF(OR(B101&lt;&gt;"",J101&lt;&gt;""),CONCATENATE(#REF!,"_",$A101,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I101="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G101" s="14" t="str">
@@ -5211,7 +5211,7 @@
         <v/>
       </c>
       <c r="H101" s="14" t="str">
-        <f>IF(AND(I101&lt;&gt;"",I101&lt;&gt;0),IF(OR(B101&lt;&gt;"",J101&lt;&gt;""),CONCATENATE(#REF!,"_",$A101,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I101" s="14" t="str">
@@ -5228,7 +5228,7 @@
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14" t="str">
-        <f>IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE(#REF!,"_",$A102,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I102="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G102" s="14" t="str">
@@ -5236,7 +5236,7 @@
         <v/>
       </c>
       <c r="H102" s="14" t="str">
-        <f>IF(AND(I102&lt;&gt;"",I102&lt;&gt;0),IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE(#REF!,"_",$A102,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I102" s="14" t="str">
@@ -5253,7 +5253,7 @@
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
       <c r="F103" s="14" t="str">
-        <f>IF(OR(B103&lt;&gt;"",J103&lt;&gt;""),CONCATENATE(#REF!,"_",$A103,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I103="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G103" s="14" t="str">
@@ -5261,7 +5261,7 @@
         <v/>
       </c>
       <c r="H103" s="14" t="str">
-        <f>IF(AND(I103&lt;&gt;"",I103&lt;&gt;0),IF(OR(B103&lt;&gt;"",J103&lt;&gt;""),CONCATENATE(#REF!,"_",$A103,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I103" s="14" t="str">
@@ -5278,7 +5278,7 @@
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
       <c r="F104" s="14" t="str">
-        <f>IF(OR(B104&lt;&gt;"",J104&lt;&gt;""),CONCATENATE(#REF!,"_",$A104,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I104="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G104" s="14" t="str">
@@ -5286,7 +5286,7 @@
         <v/>
       </c>
       <c r="H104" s="14" t="str">
-        <f>IF(AND(I104&lt;&gt;"",I104&lt;&gt;0),IF(OR(B104&lt;&gt;"",J104&lt;&gt;""),CONCATENATE(#REF!,"_",$A104,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I104" s="14" t="str">
@@ -5303,7 +5303,7 @@
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
       <c r="F105" s="14" t="str">
-        <f>IF(OR(B105&lt;&gt;"",J105&lt;&gt;""),CONCATENATE(#REF!,"_",$A105,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I105="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G105" s="14" t="str">
@@ -5311,7 +5311,7 @@
         <v/>
       </c>
       <c r="H105" s="14" t="str">
-        <f>IF(AND(I105&lt;&gt;"",I105&lt;&gt;0),IF(OR(B105&lt;&gt;"",J105&lt;&gt;""),CONCATENATE(#REF!,"_",$A105,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I105" s="14" t="str">
@@ -5328,7 +5328,7 @@
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
       <c r="F106" s="14" t="str">
-        <f>IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),CONCATENATE(#REF!,"_",$A106,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I106="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G106" s="14" t="str">
@@ -5336,7 +5336,7 @@
         <v/>
       </c>
       <c r="H106" s="14" t="str">
-        <f>IF(AND(I106&lt;&gt;"",I106&lt;&gt;0),IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),CONCATENATE(#REF!,"_",$A106,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I106" s="14" t="str">
@@ -5353,7 +5353,7 @@
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
       <c r="F107" s="14" t="str">
-        <f>IF(OR(B107&lt;&gt;"",J107&lt;&gt;""),CONCATENATE(#REF!,"_",$A107,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I107="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G107" s="14" t="str">
@@ -5361,7 +5361,7 @@
         <v/>
       </c>
       <c r="H107" s="14" t="str">
-        <f>IF(AND(I107&lt;&gt;"",I107&lt;&gt;0),IF(OR(B107&lt;&gt;"",J107&lt;&gt;""),CONCATENATE(#REF!,"_",$A107,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I107" s="14" t="str">
@@ -5378,7 +5378,7 @@
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
       <c r="F108" s="14" t="str">
-        <f>IF(OR(B108&lt;&gt;"",J108&lt;&gt;""),CONCATENATE(#REF!,"_",$A108,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I108="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G108" s="14" t="str">
@@ -5386,7 +5386,7 @@
         <v/>
       </c>
       <c r="H108" s="14" t="str">
-        <f>IF(AND(I108&lt;&gt;"",I108&lt;&gt;0),IF(OR(B108&lt;&gt;"",J108&lt;&gt;""),CONCATENATE(#REF!,"_",$A108,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I108" s="14" t="str">
@@ -5479,25 +5479,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5505,11 +5505,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="F3" s="42"/>
       <c r="H3" s="32" t="s">
         <v>18</v>
@@ -5560,11 +5560,11 @@
       <c r="C5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="110" t="str">
+      <c r="D5" s="111" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>CN_10_02_CO</v>
       </c>
-      <c r="E5" s="111"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="42"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
@@ -5609,12 +5609,12 @@
       <c r="C7" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="96" t="str">
+      <c r="D7" s="97" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_CN_10_02_CO.xls</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="H7" s="32" t="s">
         <v>24</v>
       </c>
@@ -5708,14 +5708,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="101"/>
       <c r="I13" s="32" t="s">
         <v>33</v>
       </c>
@@ -5748,12 +5748,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
       <c r="J15" s="32">
         <v>12</v>
       </c>
@@ -5793,12 +5793,12 @@
       <c r="C17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="104" t="str">
+      <c r="D17" s="105" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>CN_10_02_REC10</v>
       </c>
-      <c r="E17" s="105"/>
-      <c r="F17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107"/>
       <c r="J17" s="32">
         <v>14</v>
       </c>
@@ -5814,12 +5814,12 @@
       <c r="C18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="96" t="str">
+      <c r="D18" s="97" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_CN_10_02_REC10.xls</v>
       </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="98"/>
       <c r="J18" s="32">
         <v>15</v>
       </c>
@@ -6211,41 +6211,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="113" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="112" t="s">
+      <c r="E1" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="G1" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
       <c r="H2" s="51" t="s">
         <v>65</v>
       </c>

</xml_diff>